<commit_message>
Feat: Artefactos de Scrum
Se añade en la carpeta de Artefactos el sprint backlog, y burndown chart
</commit_message>
<xml_diff>
--- a/Sprint Backlog.xlsx
+++ b/Sprint Backlog.xlsx
@@ -5,16 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://epnecuador-my.sharepoint.com/personal/carlos_bayas_epn_edu_ec/Documents/APUNTES CJ7/7 mo Semestre/Metodologías Ágiles/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER-PC\Documents\GitHub\Proyecto-Calculadora-Scrum\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B1C48308-E7DC-4FE7-AFA3-E44464D7B5B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BD4F0F4-3102-4FDB-8026-516801508972}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{77696CBA-44D6-471E-BC5B-2422C241208C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="1" xr2:uid="{77696CBA-44D6-471E-BC5B-2422C241208C}"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
-    <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sprint 1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sprint 2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,15 +35,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="34">
   <si>
     <t>Tareas</t>
-  </si>
-  <si>
-    <t>L</t>
-  </si>
-  <si>
-    <t>M</t>
   </si>
   <si>
     <t>J</t>
@@ -119,6 +113,33 @@
   <si>
     <t>Entrega</t>
   </si>
+  <si>
+    <t>S</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>Responsable</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Freddy </t>
+  </si>
+  <si>
+    <t>Angel</t>
+  </si>
+  <si>
+    <t>Ariel</t>
+  </si>
+  <si>
+    <t>Luis</t>
+  </si>
+  <si>
+    <t>Manejar errores de priorización de Operaciones</t>
+  </si>
+  <si>
+    <t xml:space="preserve">En base a lo real: </t>
+  </si>
 </sst>
 </file>
 
@@ -188,7 +209,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -222,14 +243,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -237,9 +270,6 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -266,10 +296,41 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -282,13 +343,14 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -479,7 +541,7 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000002-5891-4A03-8366-7E93C588A24D}"/>
+                  <c16:uniqueId val="{00000000-8A12-4BEF-A99F-CCB175E31602}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
@@ -521,7 +583,7 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000003-5891-4A03-8366-7E93C588A24D}"/>
+                  <c16:uniqueId val="{00000001-8A12-4BEF-A99F-CCB175E31602}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
@@ -583,7 +645,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Hoja1!$H$13:$J$13</c:f>
+              <c:f>'Sprint 1'!$H$13:$J$13</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
@@ -600,15 +662,15 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Hoja1!$H$3:$J$3</c:f>
+              <c:f>'Sprint 1'!$H$3:$J$3</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>13</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>7</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -619,7 +681,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-5891-4A03-8366-7E93C588A24D}"/>
+              <c16:uniqueId val="{00000002-8A12-4BEF-A99F-CCB175E31602}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -716,7 +778,7 @@
             <c:bubble3D val="0"/>
             <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000008-5891-4A03-8366-7E93C588A24D}"/>
+                <c16:uniqueId val="{00000003-8A12-4BEF-A99F-CCB175E31602}"/>
               </c:ext>
             </c:extLst>
           </c:dPt>
@@ -738,7 +800,7 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000009-5891-4A03-8366-7E93C588A24D}"/>
+                  <c16:uniqueId val="{00000004-8A12-4BEF-A99F-CCB175E31602}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
@@ -748,7 +810,7 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{0000000A-5891-4A03-8366-7E93C588A24D}"/>
+                  <c16:uniqueId val="{00000005-8A12-4BEF-A99F-CCB175E31602}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
@@ -810,7 +872,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Hoja1!$H$13:$J$13</c:f>
+              <c:f>'Sprint 1'!$H$13:$J$13</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
@@ -827,15 +889,15 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Hoja1!$H$14:$J$14</c:f>
+              <c:f>'Sprint 1'!$H$14:$J$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>11</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>8</c:v>
+                  <c:v>21</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -846,7 +908,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000007-5891-4A03-8366-7E93C588A24D}"/>
+              <c16:uniqueId val="{00000006-8A12-4BEF-A99F-CCB175E31602}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1327,7 +1389,7 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000005-D6C2-4735-BF98-19AF1DAC3885}"/>
+                  <c16:uniqueId val="{00000000-6BD5-4ED2-A2D5-B822447EAB87}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
@@ -1349,7 +1411,7 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000007-D6C2-4735-BF98-19AF1DAC3885}"/>
+                  <c16:uniqueId val="{00000001-6BD5-4ED2-A2D5-B822447EAB87}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
@@ -1399,7 +1461,7 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000009-D6C2-4735-BF98-19AF1DAC3885}"/>
+                  <c16:uniqueId val="{00000002-6BD5-4ED2-A2D5-B822447EAB87}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
@@ -1464,7 +1526,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Hoja2!$G$2:$I$2</c:f>
+              <c:f>'Sprint 2'!$G$2:$I$2</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
@@ -1481,15 +1543,15 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Hoja2!$G$3:$I$3</c:f>
+              <c:f>'Sprint 2'!$G$3:$I$3</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>10</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>6</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -1500,7 +1562,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-D6C2-4735-BF98-19AF1DAC3885}"/>
+              <c16:uniqueId val="{00000003-6BD5-4ED2-A2D5-B822447EAB87}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1586,7 +1648,29 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000006-D6C2-4735-BF98-19AF1DAC3885}"/>
+                  <c16:uniqueId val="{00000004-6BD5-4ED2-A2D5-B822447EAB87}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-5.1037500368092306E-2"/>
+                  <c:y val="8.1215355772853437E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000008-6BD5-4ED2-A2D5-B822447EAB87}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
@@ -1596,7 +1680,7 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000008-D6C2-4735-BF98-19AF1DAC3885}"/>
+                  <c16:uniqueId val="{00000005-6BD5-4ED2-A2D5-B822447EAB87}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
@@ -1659,7 +1743,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Hoja2!$G$2:$I$2</c:f>
+              <c:f>'Sprint 2'!$G$2:$I$2</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
@@ -1676,15 +1760,15 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Hoja2!$G$14:$I$14</c:f>
+              <c:f>'Sprint 2'!$G$14:$I$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>9</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>9</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -1695,7 +1779,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-D6C2-4735-BF98-19AF1DAC3885}"/>
+              <c16:uniqueId val="{00000006-6BD5-4ED2-A2D5-B822447EAB87}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -3151,26 +3235,28 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>726469</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>34472</xdr:rowOff>
+      <xdr:colOff>1287518</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>131470</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>5286590</xdr:colOff>
-      <xdr:row>36</xdr:row>
-      <xdr:rowOff>56243</xdr:rowOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>400812</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>181427</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="7" name="Gráfico 6">
+        <xdr:cNvPr id="5" name="Gráfico 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{17B7E0B5-80A7-472C-81BE-85B813F83E45}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{43D30631-3BD7-46E4-B3EF-9A4965D6A202}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
@@ -3191,7 +3277,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
+      <xdr:col>7</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>4</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -3234,7 +3320,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
+      <xdr:col>7</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>4</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -3278,26 +3364,28 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>666597</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>133612</xdr:rowOff>
+      <xdr:colOff>1112347</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>168232</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>5288162</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>173771</xdr:rowOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>5508</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>14097</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="5" name="Gráfico 4">
+        <xdr:cNvPr id="6" name="Gráfico 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{544D6F96-CF42-46BB-9C64-E04A0F75884A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2DF4483B-F773-42A2-BDC1-878014F70BDB}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
@@ -3611,10 +3699,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E541A42A-4D29-439E-A605-99F41F004E2C}">
-  <dimension ref="A1:J29"/>
+  <dimension ref="A1:J73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="63" zoomScaleNormal="84" workbookViewId="0">
-      <selection activeCell="H27" sqref="H27"/>
+    <sheetView topLeftCell="A11" zoomScale="60" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="I49" sqref="I49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3622,7 +3710,9 @@
     <col min="1" max="1" width="82.7109375" customWidth="1"/>
     <col min="2" max="2" width="7.140625" customWidth="1"/>
     <col min="3" max="3" width="6.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="6" width="4.7109375" customWidth="1"/>
+    <col min="4" max="4" width="5.85546875" customWidth="1"/>
+    <col min="5" max="5" width="14.28515625" customWidth="1"/>
+    <col min="6" max="6" width="4.7109375" customWidth="1"/>
     <col min="7" max="7" width="16.42578125" customWidth="1"/>
     <col min="8" max="8" width="8.28515625" customWidth="1"/>
     <col min="9" max="9" width="8.42578125" customWidth="1"/>
@@ -3631,321 +3721,618 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A1" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
+      <c r="A1" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="4"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="36" t="s">
+        <v>27</v>
+      </c>
+      <c r="G2" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="H2" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="I2" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="J2" s="19" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="25" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="26" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="30">
+        <v>3</v>
+      </c>
+      <c r="D3" s="30">
+        <v>3</v>
+      </c>
+      <c r="E3" s="22" t="s">
+        <v>28</v>
+      </c>
+      <c r="G3" s="1">
+        <v>40</v>
+      </c>
+      <c r="H3" s="1">
+        <v>20</v>
+      </c>
+      <c r="I3" s="1">
+        <v>20</v>
+      </c>
+      <c r="J3" s="20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="12" t="s">
+      <c r="B4" s="26">
+        <v>1</v>
+      </c>
+      <c r="C4" s="30">
+        <v>4</v>
+      </c>
+      <c r="D4" s="30">
+        <v>4</v>
+      </c>
+      <c r="E4" s="22" t="s">
+        <v>28</v>
+      </c>
+      <c r="G4" s="4"/>
+      <c r="H4" s="4"/>
+      <c r="I4" s="4"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="25" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="26">
+        <v>1</v>
+      </c>
+      <c r="C5" s="30">
         <v>3</v>
       </c>
-      <c r="D2" s="12" t="s">
+      <c r="D5" s="30">
+        <v>3</v>
+      </c>
+      <c r="E5" s="22" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="25" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="26">
+        <v>2</v>
+      </c>
+      <c r="C6" s="30">
+        <v>2</v>
+      </c>
+      <c r="D6" s="30">
+        <v>2</v>
+      </c>
+      <c r="E6" s="22" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="26">
+        <v>3</v>
+      </c>
+      <c r="C7" s="30">
+        <v>2</v>
+      </c>
+      <c r="D7" s="30">
+        <v>2</v>
+      </c>
+      <c r="E7" s="22" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="25" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" s="26">
+        <v>1</v>
+      </c>
+      <c r="C8" s="30">
+        <v>2</v>
+      </c>
+      <c r="D8" s="30">
+        <v>2</v>
+      </c>
+      <c r="E8" s="22" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" s="26">
         <v>4</v>
       </c>
-      <c r="G2" s="12" t="s">
+      <c r="C9" s="32">
+        <v>2</v>
+      </c>
+      <c r="D9" s="32">
+        <v>2</v>
+      </c>
+      <c r="E9" s="22" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="28" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" s="24" t="s">
+        <v>17</v>
+      </c>
+      <c r="C10" s="24">
+        <v>2</v>
+      </c>
+      <c r="D10" s="24">
+        <v>2</v>
+      </c>
+      <c r="E10" s="22" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B11" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" s="17">
+        <f>SUM(C3:C10)</f>
+        <v>20</v>
+      </c>
+      <c r="D11" s="33">
+        <f>SUM(D3:D10)</f>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="G13" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="H13" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="I13" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="H2" s="12" t="s">
+      <c r="J13" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="I2" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="J2" s="24" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="7" t="s">
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B14" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="C14" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="D14" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="G14" s="1">
+        <v>40</v>
+      </c>
+      <c r="H14" s="1">
+        <v>19</v>
+      </c>
+      <c r="I14" s="1">
+        <v>21</v>
+      </c>
+      <c r="J14" s="20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" s="25" t="s">
+        <v>4</v>
+      </c>
+      <c r="B15" s="26" t="s">
+        <v>9</v>
+      </c>
+      <c r="C15" s="30">
+        <v>3</v>
+      </c>
+      <c r="D15" s="30">
+        <v>3</v>
+      </c>
+      <c r="E15" s="22" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" s="25" t="s">
+        <v>5</v>
+      </c>
+      <c r="B16" s="26">
+        <v>1</v>
+      </c>
+      <c r="C16" s="30">
+        <v>4</v>
+      </c>
+      <c r="D16" s="30">
+        <v>4</v>
+      </c>
+      <c r="E16" s="22" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" s="19">
+      <c r="B17" s="26">
+        <v>1</v>
+      </c>
+      <c r="C17" s="30">
         <v>3</v>
       </c>
-      <c r="D3" s="19">
+      <c r="D17" s="30">
+        <v>3</v>
+      </c>
+      <c r="E17" s="22" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="25" t="s">
+        <v>7</v>
+      </c>
+      <c r="B18" s="26">
+        <v>2</v>
+      </c>
+      <c r="C18" s="30">
+        <v>2</v>
+      </c>
+      <c r="D18" s="30">
+        <v>2</v>
+      </c>
+      <c r="E18" s="22" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="B19" s="26">
+        <v>3</v>
+      </c>
+      <c r="C19" s="30">
+        <v>2</v>
+      </c>
+      <c r="D19" s="30">
+        <v>2</v>
+      </c>
+      <c r="E19" s="22" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="25" t="s">
+        <v>19</v>
+      </c>
+      <c r="B20" s="26">
         <v>1</v>
       </c>
-      <c r="G3" s="1">
-        <v>20</v>
-      </c>
-      <c r="H3" s="1">
+      <c r="C20" s="30">
+        <v>2</v>
+      </c>
+      <c r="D20" s="30">
+        <v>2</v>
+      </c>
+      <c r="E20" s="22" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="25" t="s">
         <v>13</v>
       </c>
-      <c r="I3" s="1">
-        <v>7</v>
-      </c>
-      <c r="J3" s="25">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" s="8">
-        <v>6</v>
-      </c>
-      <c r="C4" s="19">
+      <c r="B21" s="26">
+        <v>4</v>
+      </c>
+      <c r="C21" s="32">
+        <v>1</v>
+      </c>
+      <c r="D21" s="32">
+        <v>1</v>
+      </c>
+      <c r="E21" s="22" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="28" t="s">
+        <v>16</v>
+      </c>
+      <c r="B22" s="24" t="s">
+        <v>17</v>
+      </c>
+      <c r="C22" s="24">
         <v>2</v>
       </c>
-      <c r="D4" s="19">
-        <v>1</v>
-      </c>
-      <c r="G4" s="5"/>
-      <c r="H4" s="5"/>
-      <c r="I4" s="5"/>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" s="8">
-        <v>1</v>
-      </c>
-      <c r="C5" s="19">
-        <v>3</v>
-      </c>
-      <c r="D5" s="19">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" s="8">
-        <v>2</v>
-      </c>
-      <c r="C6" s="19">
-        <v>1</v>
-      </c>
-      <c r="D6" s="19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7" s="8">
-        <v>3</v>
-      </c>
-      <c r="C7" s="19">
-        <v>1</v>
-      </c>
-      <c r="D7" s="19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="7" t="s">
+      <c r="D22" s="24">
+        <v>4</v>
+      </c>
+      <c r="E22" s="22" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="21"/>
+      <c r="B23" s="29" t="s">
+        <v>18</v>
+      </c>
+      <c r="C23" s="33">
+        <f>SUM(C15:C22)</f>
+        <v>19</v>
+      </c>
+      <c r="D23" s="33">
+        <f>SUM(D15:D22)</f>
         <v>21</v>
       </c>
-      <c r="B8" s="8">
-        <v>9</v>
-      </c>
-      <c r="C8" s="19">
-        <v>1</v>
-      </c>
-      <c r="D8" s="19">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="C9" s="21">
-        <v>2</v>
-      </c>
-      <c r="D9" s="21">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B10" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="C10" s="22">
-        <f>SUM(C3:C9)</f>
-        <v>13</v>
-      </c>
-      <c r="D10" s="22">
-        <f>SUM(D3:D9)</f>
-        <v>7</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="23" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="B13" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="C13" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="D13" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="G13" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="H13" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="I13" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="J13" s="24" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="B14" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="C14" s="19">
-        <v>2</v>
-      </c>
-      <c r="D14" s="19">
-        <v>2</v>
-      </c>
-      <c r="G14" s="1">
-        <v>20</v>
-      </c>
-      <c r="H14" s="1">
-        <v>11</v>
-      </c>
-      <c r="I14" s="1">
-        <v>8</v>
-      </c>
-      <c r="J14" s="25">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B15" s="8">
-        <v>6</v>
-      </c>
-      <c r="C15" s="19">
-        <v>1</v>
-      </c>
-      <c r="D15" s="19">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="B16" s="8">
-        <v>1</v>
-      </c>
-      <c r="C16" s="19">
-        <v>2</v>
-      </c>
-      <c r="D16" s="19">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="B17" s="8">
-        <v>2</v>
-      </c>
-      <c r="C17" s="19">
-        <v>1</v>
-      </c>
-      <c r="D17" s="19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B18" s="8">
-        <v>3</v>
-      </c>
-      <c r="C18" s="19">
-        <v>1</v>
-      </c>
-      <c r="D18" s="19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="B19" s="8">
-        <v>9</v>
-      </c>
-      <c r="C19" s="19">
-        <v>1</v>
-      </c>
-      <c r="D19" s="19">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="B20" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="C20" s="21">
-        <v>3</v>
-      </c>
-      <c r="D20" s="21">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B21" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="C21" s="22">
-        <f>SUM(C14:C20)</f>
-        <v>11</v>
-      </c>
-      <c r="D21" s="22">
-        <f>SUM(D14:D20)</f>
-        <v>9</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D29" s="2"/>
+      <c r="E23" s="21"/>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" s="21"/>
+      <c r="B46" s="21"/>
+      <c r="C46" s="21"/>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" s="21"/>
+      <c r="B47" s="21"/>
+      <c r="C47" s="21"/>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" s="21"/>
+      <c r="B48" s="21"/>
+      <c r="C48" s="21"/>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A49" s="21"/>
+      <c r="B49" s="21"/>
+      <c r="C49" s="21"/>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A50" s="21"/>
+      <c r="B50" s="21"/>
+      <c r="C50" s="21"/>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A51" s="21"/>
+      <c r="B51" s="21"/>
+      <c r="C51" s="21"/>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A52" s="21"/>
+      <c r="B52" s="21"/>
+      <c r="C52" s="21"/>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A53" s="21"/>
+      <c r="B53" s="21"/>
+      <c r="C53" s="21"/>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A54" s="21"/>
+      <c r="B54" s="21"/>
+      <c r="C54" s="21"/>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A55" s="21"/>
+      <c r="B55" s="21"/>
+      <c r="C55" s="21"/>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A56" s="21"/>
+      <c r="B56" s="21"/>
+      <c r="C56" s="21"/>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A57" s="21"/>
+      <c r="B57" s="21"/>
+      <c r="C57" s="21"/>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A58" s="21"/>
+      <c r="B58" s="21"/>
+      <c r="C58" s="21"/>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A60" s="21"/>
+      <c r="B60" s="21"/>
+      <c r="C60" s="21"/>
+      <c r="D60" s="21"/>
+      <c r="E60" s="21"/>
+      <c r="F60" s="21"/>
+      <c r="G60" s="21"/>
+      <c r="H60" s="21"/>
+      <c r="I60" s="21"/>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A61" s="21"/>
+      <c r="B61" s="21"/>
+      <c r="C61" s="21"/>
+      <c r="D61" s="21"/>
+      <c r="E61" s="21"/>
+      <c r="F61" s="21"/>
+      <c r="G61" s="21"/>
+      <c r="H61" s="21"/>
+      <c r="I61" s="21"/>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A62" s="21"/>
+      <c r="B62" s="21"/>
+      <c r="C62" s="21"/>
+      <c r="D62" s="21"/>
+      <c r="E62" s="21"/>
+      <c r="F62" s="21"/>
+      <c r="G62" s="21"/>
+      <c r="H62" s="21"/>
+      <c r="I62" s="21"/>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A63" s="21"/>
+      <c r="B63" s="21"/>
+      <c r="C63" s="21"/>
+      <c r="D63" s="21"/>
+      <c r="E63" s="21"/>
+      <c r="F63" s="21"/>
+      <c r="G63" s="21"/>
+      <c r="H63" s="21"/>
+      <c r="I63" s="21"/>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A64" s="21"/>
+      <c r="B64" s="21"/>
+      <c r="C64" s="21"/>
+      <c r="D64" s="21"/>
+      <c r="E64" s="21"/>
+      <c r="F64" s="21"/>
+      <c r="G64" s="21"/>
+      <c r="H64" s="21"/>
+      <c r="I64" s="21"/>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A65" s="21"/>
+      <c r="B65" s="21"/>
+      <c r="C65" s="21"/>
+      <c r="D65" s="21"/>
+      <c r="E65" s="21"/>
+      <c r="F65" s="21"/>
+      <c r="G65" s="21"/>
+      <c r="H65" s="21"/>
+      <c r="I65" s="21"/>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A66" s="21"/>
+      <c r="B66" s="21"/>
+      <c r="C66" s="21"/>
+      <c r="D66" s="21"/>
+      <c r="E66" s="21"/>
+      <c r="F66" s="21"/>
+      <c r="G66" s="21"/>
+      <c r="H66" s="21"/>
+      <c r="I66" s="21"/>
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A67" s="21"/>
+      <c r="B67" s="21"/>
+      <c r="C67" s="21"/>
+      <c r="D67" s="21"/>
+      <c r="E67" s="21"/>
+      <c r="F67" s="21"/>
+      <c r="G67" s="21"/>
+      <c r="H67" s="21"/>
+      <c r="I67" s="21"/>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A68" s="21"/>
+      <c r="B68" s="21"/>
+      <c r="C68" s="21"/>
+      <c r="D68" s="21"/>
+      <c r="E68" s="21"/>
+      <c r="F68" s="21"/>
+      <c r="G68" s="21"/>
+      <c r="H68" s="21"/>
+      <c r="I68" s="21"/>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A69" s="21"/>
+      <c r="B69" s="21"/>
+      <c r="C69" s="21"/>
+      <c r="D69" s="21"/>
+      <c r="E69" s="21"/>
+      <c r="F69" s="21"/>
+      <c r="G69" s="21"/>
+      <c r="H69" s="21"/>
+      <c r="I69" s="21"/>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A70" s="21"/>
+      <c r="B70" s="21"/>
+      <c r="C70" s="21"/>
+      <c r="D70" s="21"/>
+      <c r="E70" s="21"/>
+      <c r="F70" s="21"/>
+      <c r="G70" s="21"/>
+      <c r="H70" s="21"/>
+      <c r="I70" s="21"/>
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A71" s="21"/>
+      <c r="B71" s="21"/>
+      <c r="C71" s="21"/>
+      <c r="D71" s="21"/>
+      <c r="E71" s="21"/>
+      <c r="F71" s="21"/>
+      <c r="G71" s="21"/>
+      <c r="H71" s="21"/>
+      <c r="I71" s="21"/>
+    </row>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A72" s="21"/>
+      <c r="B72" s="21"/>
+      <c r="C72" s="21"/>
+      <c r="D72" s="21"/>
+      <c r="E72" s="21"/>
+      <c r="F72" s="21"/>
+      <c r="G72" s="21"/>
+      <c r="H72" s="21"/>
+      <c r="I72" s="21"/>
+    </row>
+    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A73" s="21"/>
+      <c r="B73" s="21"/>
+      <c r="C73" s="21"/>
+      <c r="D73" s="21"/>
+      <c r="E73" s="21"/>
+      <c r="F73" s="21"/>
+      <c r="G73" s="21"/>
+      <c r="H73" s="21"/>
+      <c r="I73" s="21"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3955,10 +4342,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B8CFFCB-50ED-4139-B1FC-A23BD20D8731}">
-  <dimension ref="A1:I18"/>
+  <dimension ref="A1:J20"/>
   <sheetViews>
-    <sheetView zoomScale="67" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="I27" sqref="I27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3968,266 +4355,298 @@
     <col min="6" max="6" width="11.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A1" s="13" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="9" t="s">
+    <row r="1" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="A1" s="11" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="H2" s="27" t="s">
+        <v>23</v>
+      </c>
+      <c r="I2" s="27" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="6">
         <v>5</v>
       </c>
-      <c r="C2" s="10" t="s">
+      <c r="C3" s="15">
+        <v>3</v>
+      </c>
+      <c r="D3" s="15">
+        <v>2</v>
+      </c>
+      <c r="F3" s="1">
+        <v>29</v>
+      </c>
+      <c r="G3" s="1">
+        <v>15</v>
+      </c>
+      <c r="H3" s="22">
+        <v>14</v>
+      </c>
+      <c r="I3" s="37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B4" s="6">
+        <v>5</v>
+      </c>
+      <c r="C4" s="15">
+        <v>2</v>
+      </c>
+      <c r="D4" s="15">
+        <v>3</v>
+      </c>
+      <c r="H4" s="4"/>
+      <c r="I4" s="4"/>
+      <c r="J4" s="4"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="6">
+        <v>6</v>
+      </c>
+      <c r="C5" s="15">
+        <v>2</v>
+      </c>
+      <c r="D5" s="15">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="25" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" s="6">
+        <v>7</v>
+      </c>
+      <c r="C6" s="15">
+        <v>2</v>
+      </c>
+      <c r="D6" s="15">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" s="4">
+        <v>8</v>
+      </c>
+      <c r="C7" s="16">
+        <v>3</v>
+      </c>
+      <c r="D7" s="16">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" s="24" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" s="22">
+        <v>3</v>
+      </c>
+      <c r="D8" s="22">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="28"/>
+      <c r="B9" s="34" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" s="35">
+        <f>SUM(C3:C8)</f>
+        <v>15</v>
+      </c>
+      <c r="D9" s="35">
+        <f>SUM(D3:D8)</f>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="2"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="3"/>
+      <c r="B11" s="3"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B13" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="D13" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="F13" s="27" t="s">
+        <v>21</v>
+      </c>
+      <c r="G13" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="H13" s="27" t="s">
+        <v>23</v>
+      </c>
+      <c r="I13" s="27" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" s="25" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14" s="26">
+        <v>5</v>
+      </c>
+      <c r="C14" s="30">
+        <v>3</v>
+      </c>
+      <c r="D14" s="30">
+        <v>2</v>
+      </c>
+      <c r="F14" s="22">
+        <v>29</v>
+      </c>
+      <c r="G14" s="22">
+        <v>17</v>
+      </c>
+      <c r="H14" s="22">
+        <v>12</v>
+      </c>
+      <c r="I14" s="37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" s="25" t="s">
+        <v>32</v>
+      </c>
+      <c r="B15" s="26">
+        <v>5</v>
+      </c>
+      <c r="C15" s="30">
+        <v>3</v>
+      </c>
+      <c r="D15" s="30">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" s="25" t="s">
+        <v>14</v>
+      </c>
+      <c r="B16" s="26">
+        <v>6</v>
+      </c>
+      <c r="C16" s="30">
+        <v>2</v>
+      </c>
+      <c r="D16" s="30">
         <v>1</v>
       </c>
-      <c r="D2" s="10" t="s">
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="25" t="s">
+        <v>19</v>
+      </c>
+      <c r="B17" s="26">
+        <v>7</v>
+      </c>
+      <c r="C17" s="30">
         <v>2</v>
       </c>
-      <c r="F2" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="G2" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="H2" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="I2" s="9" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="B3" s="8">
-        <v>5</v>
-      </c>
-      <c r="C3" s="19">
+      <c r="D17" s="30">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="B18" s="23">
+        <v>8</v>
+      </c>
+      <c r="C18" s="31">
+        <v>4</v>
+      </c>
+      <c r="D18" s="31">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="28" t="s">
+        <v>16</v>
+      </c>
+      <c r="B19" s="24" t="s">
+        <v>17</v>
+      </c>
+      <c r="C19" s="22">
         <v>3</v>
       </c>
-      <c r="D3" s="19">
-        <v>2</v>
-      </c>
-      <c r="F3" s="1">
-        <v>16</v>
-      </c>
-      <c r="G3" s="1">
-        <v>10</v>
-      </c>
-      <c r="H3" s="1">
-        <v>6</v>
-      </c>
-      <c r="I3" s="25">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="B4" s="8">
-        <v>4</v>
-      </c>
-      <c r="C4" s="19">
-        <v>2</v>
-      </c>
-      <c r="D4" s="19">
-        <v>1</v>
-      </c>
-      <c r="F4" s="5"/>
-      <c r="G4" s="5"/>
-      <c r="H4" s="5"/>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="B5" s="8">
-        <v>6</v>
-      </c>
-      <c r="C5" s="19">
-        <v>1</v>
-      </c>
-      <c r="D5" s="19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="7" t="s">
+      <c r="D19" s="22">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="28"/>
+      <c r="B20" s="34" t="s">
+        <v>18</v>
+      </c>
+      <c r="C20" s="35">
+        <f>SUM(C14:C19)</f>
         <v>17</v>
       </c>
-      <c r="B6" s="8">
-        <v>10</v>
-      </c>
-      <c r="C6" s="19">
-        <v>2</v>
-      </c>
-      <c r="D6" s="19">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="C7" s="20">
-        <v>2</v>
-      </c>
-      <c r="D7" s="20">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B8" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="C8" s="18">
-        <f>SUM(C3:C7)</f>
-        <v>10</v>
-      </c>
-      <c r="D8" s="18">
-        <f>SUM(D3:D7)</f>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="3"/>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="4"/>
-      <c r="B11" s="4"/>
-      <c r="C11" s="4"/>
-      <c r="D11" s="4"/>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="B12" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="C12" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="D12" s="10" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="B13" s="8">
-        <v>5</v>
-      </c>
-      <c r="C13" s="19">
-        <v>2</v>
-      </c>
-      <c r="D13" s="19">
-        <v>1</v>
-      </c>
-      <c r="F13" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="G13" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="H13" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="I13" s="9" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="B14" s="8">
-        <v>4</v>
-      </c>
-      <c r="C14" s="19">
-        <v>2</v>
-      </c>
-      <c r="D14" s="19">
-        <v>1</v>
-      </c>
-      <c r="F14" s="1">
-        <v>16</v>
-      </c>
-      <c r="G14" s="1">
-        <v>9</v>
-      </c>
-      <c r="H14" s="1">
-        <v>9</v>
-      </c>
-      <c r="I14" s="25">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="B15" s="8">
-        <v>6</v>
-      </c>
-      <c r="C15" s="19">
-        <v>1</v>
-      </c>
-      <c r="D15" s="19">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="B16" s="8">
-        <v>10</v>
-      </c>
-      <c r="C16" s="19">
-        <v>2</v>
-      </c>
-      <c r="D16" s="19">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="B17" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="C17" s="20">
-        <v>2</v>
-      </c>
-      <c r="D17" s="20">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B18" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="C18" s="18">
-        <f>SUM(C13:C17)</f>
-        <v>9</v>
-      </c>
-      <c r="D18" s="18">
-        <f>SUM(D13:D17)</f>
-        <v>9</v>
+      <c r="D20" s="35">
+        <f>SUM(D14:D19)</f>
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>